<commit_message>
aact-784:  Refactor so that we will be able to retrieve multiple sheets from the Data Definitions spreadsheet.
</commit_message>
<xml_diff>
--- a/public/data_definitions/proj_anderson.xlsx
+++ b/public/data_definitions/proj_anderson.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="5360" windowWidth="25300" windowHeight="11180"/>
+    <workbookView xWindow="620" yWindow="3120" windowWidth="25300" windowHeight="11180"/>
   </bookViews>
   <sheets>
-    <sheet name="Data Dictionary" sheetId="2" r:id="rId1"/>
+    <sheet name="Data Definitions" sheetId="2" r:id="rId1"/>
     <sheet name="General Info" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="130407"/>
@@ -1391,7 +1391,7 @@
   <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:XFD32"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -2254,6 +2254,7 @@
     <row r="57" spans="1:5" ht="70"/>
     <row r="60" spans="1:5" ht="42"/>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="2">
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B25:E25"/>
@@ -2278,6 +2279,11 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="95.5" customWidth="1"/>
+    <col min="6" max="6" width="25.5" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -2322,9 +2328,10 @@
       <c r="C6" s="1"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="75" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>

</xml_diff>